<commit_message>
Fixed CHE release typos
This fixed version was sent to Calla, corrected typos in BOM and fab
readme. Retagging as release.
</commit_message>
<xml_diff>
--- a/Codeshelf-0005-recovered/CS0005.ECO.xlsx
+++ b/Codeshelf-0005-recovered/CS0005.ECO.xlsx
@@ -54,9 +54,6 @@
     <t>Not required for programming adapter</t>
   </si>
   <si>
-    <t>Change J5-LCD-3V3</t>
-  </si>
-  <si>
     <t>Header interferes with LCD assembly</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Original part unavailable, make suitable substitution (last time FDD5614P)</t>
+  </si>
+  <si>
+    <t>Change J5-LCD-3V3 to DNP</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,26 +488,26 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>